<commit_message>
aggiunta relazione sensori temperatura, e altri dati analizzati, altre modifiche minori
</commit_message>
<xml_diff>
--- a/Sensore_temp/dati_graph.xlsx
+++ b/Sensore_temp/dati_graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Esame\Documents\Arduino\Sketches\PROGETTI\Sensore_temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BBB31C9-145B-4DED-88A2-225643D96DD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D125354-1A52-4423-A66C-AAF88FEB1AA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{609B357A-085B-4CB2-8DE8-5AC2C629CFDA}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="sensors_data" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">sensors_data!$B$1</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">sensors_data!$B$2:$B$151</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">sensors_data!$B$2:$B$151</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">sensors_data!$D$1</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">sensors_data!$D$2:$D$151</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">sensors_data!$C$1</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">sensors_data!$C$2:$C$151</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">sensors_data!$D$2:$D$151</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">sensors_data!$C$1</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">sensors_data!$C$2:$C$151</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">sensors_data!$D$1</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">sensors_data!$B$1</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">sensors_data!$B$2:$B$151</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">sensors_data!$B$2:$B$151</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">sensors_data!$C$2:$C$151</definedName>
     <definedName name="_xlchart.v1.8" hidden="1">sensors_data!$D$2:$D$151</definedName>
     <definedName name="DatiEsterni_1" localSheetId="0" hidden="1">sensors_data!$A$1:$D$151</definedName>
   </definedNames>
@@ -2357,17 +2357,17 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.6</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.7</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.4</cx:f>
+        <cx:f>_xlchart.v1.8</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -2442,7 +2442,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -2480,7 +2480,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{71EF0E87-7E26-4E57-BAC6-01F52993A12C}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.0</cx:f>
+              <cx:f>_xlchart.v1.4</cx:f>
               <cx:v>NTC</cx:v>
             </cx:txData>
           </cx:tx>
@@ -2511,7 +2511,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.6</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -2549,7 +2549,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{11CDE56D-2161-4EAC-97D2-0C3BE3E389E9}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.5</cx:f>
+              <cx:f>_xlchart.v1.2</cx:f>
               <cx:v>DHT11</cx:v>
             </cx:txData>
           </cx:tx>
@@ -2580,7 +2580,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.8</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -2618,7 +2618,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{8DF72453-9141-4477-A4D1-819D601B3764}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.7</cx:f>
+              <cx:f>_xlchart.v1.0</cx:f>
               <cx:v>THERMO</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5441,7 +5441,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="8374380" y="87630"/>
+              <a:off x="7505700" y="87630"/>
               <a:ext cx="4572000" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -5461,7 +5461,7 @@
             <a:lstStyle/>
             <a:p>
               <a:r>
-                <a:rPr lang="en-US" sz="1100"/>
+                <a:rPr lang="it-IT" sz="1100"/>
                 <a:t>Il grafico non è disponibile in questa versione di Excel.
 Se si modifica questa forma o si salva la cartella di lavoro in un formato di file diverso, il grafico verrà danneggiato in modo permanente.</a:t>
               </a:r>
@@ -5555,7 +5555,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3741420" y="2975610"/>
+              <a:off x="2872740" y="2975610"/>
               <a:ext cx="3086100" cy="1870710"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -5575,7 +5575,7 @@
             <a:lstStyle/>
             <a:p>
               <a:r>
-                <a:rPr lang="en-US" sz="1100"/>
+                <a:rPr lang="it-IT" sz="1100"/>
                 <a:t>Il grafico non è disponibile in questa versione di Excel.
 Se si modifica questa forma o si salva la cartella di lavoro in un formato di file diverso, il grafico verrà danneggiato in modo permanente.</a:t>
               </a:r>
@@ -5633,7 +5633,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="6964680" y="2983230"/>
+              <a:off x="6096000" y="2983230"/>
               <a:ext cx="2941320" cy="1840230"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -5653,7 +5653,7 @@
             <a:lstStyle/>
             <a:p>
               <a:r>
-                <a:rPr lang="en-US" sz="1100"/>
+                <a:rPr lang="it-IT" sz="1100"/>
                 <a:t>Il grafico non è disponibile in questa versione di Excel.
 Se si modifica questa forma o si salva la cartella di lavoro in un formato di file diverso, il grafico verrà danneggiato in modo permanente.</a:t>
               </a:r>
@@ -5711,7 +5711,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="10005060" y="2960370"/>
+              <a:off x="9136380" y="2960370"/>
               <a:ext cx="2956560" cy="1901190"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -5731,7 +5731,7 @@
             <a:lstStyle/>
             <a:p>
               <a:r>
-                <a:rPr lang="en-US" sz="1100"/>
+                <a:rPr lang="it-IT" sz="1100"/>
                 <a:t>Il grafico non è disponibile in questa versione di Excel.
 Se si modifica questa forma o si salva la cartella di lavoro in un formato di file diverso, il grafico verrà danneggiato in modo permanente.</a:t>
               </a:r>
@@ -6091,7 +6091,7 @@
   <dimension ref="A1:D151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D1048576"/>
+      <selection activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>